<commit_message>
edited "D" in .xlsx file to reflect 'gr1` and updated .R file.
</commit_message>
<xml_diff>
--- a/data/Guana_Nut_Run_Master_2019_2020.xlsx
+++ b/data/Guana_Nut_Run_Master_2019_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dunnigan_S\Desktop\OPEN_PROJECTS\guana\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE912A5-30AF-496F-86DB-FC9175B452F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD3A245-D546-4F69-9982-3EFB5F5E48EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-4740" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="338">
   <si>
     <t>DATE</t>
   </si>
@@ -736,9 +736,6 @@
   </si>
   <si>
     <t>bottom</t>
-  </si>
-  <si>
-    <t>D</t>
   </si>
   <si>
     <t>Feb 2020 Temp</t>
@@ -23556,7 +23553,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48:C181"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23591,7 +23588,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>7</v>
@@ -25193,7 +25190,7 @@
         <v>0.37561342592592589</v>
       </c>
       <c r="C22" t="s">
-        <v>233</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -25732,7 +25729,7 @@
         <v>0.60296296296296303</v>
       </c>
       <c r="C29" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D29" t="s">
         <v>24</v>
@@ -27195,7 +27192,7 @@
         <v>0.65077546296296296</v>
       </c>
       <c r="C48" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D48" t="s">
         <v>24</v>
@@ -27965,7 +27962,7 @@
         <v>0.64741898148148147</v>
       </c>
       <c r="C58" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D58" t="s">
         <v>24</v>
@@ -28735,7 +28732,7 @@
         <v>0.6312268518518519</v>
       </c>
       <c r="C68" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D68" t="s">
         <v>24</v>
@@ -30044,7 +30041,7 @@
         <v>0.63501157407407405</v>
       </c>
       <c r="C85" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D85" t="s">
         <v>24</v>
@@ -31045,7 +31042,7 @@
         <v>0.61812500000000004</v>
       </c>
       <c r="C98" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D98" t="s">
         <v>24</v>
@@ -32354,7 +32351,7 @@
         <v>0.61655092592592597</v>
       </c>
       <c r="C115" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D115" t="s">
         <v>24</v>
@@ -33740,7 +33737,7 @@
         <v>0.52651620370370367</v>
       </c>
       <c r="C133" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D133" t="s">
         <v>24</v>
@@ -33823,7 +33820,7 @@
         <v>24</v>
       </c>
       <c r="E134" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F134" t="s">
         <v>204</v>
@@ -33900,10 +33897,10 @@
         <v>24</v>
       </c>
       <c r="E135" t="s">
+        <v>250</v>
+      </c>
+      <c r="F135" t="s">
         <v>251</v>
-      </c>
-      <c r="F135" t="s">
-        <v>252</v>
       </c>
       <c r="G135">
         <v>765.9</v>
@@ -33977,10 +33974,10 @@
         <v>24</v>
       </c>
       <c r="E136" t="s">
+        <v>252</v>
+      </c>
+      <c r="F136" t="s">
         <v>253</v>
-      </c>
-      <c r="F136" t="s">
-        <v>254</v>
       </c>
       <c r="G136">
         <v>765.9</v>
@@ -34054,10 +34051,10 @@
         <v>24</v>
       </c>
       <c r="E137" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F137" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G137">
         <v>766</v>
@@ -34285,7 +34282,7 @@
         <v>24</v>
       </c>
       <c r="E140" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F140" t="s">
         <v>210</v>
@@ -34362,10 +34359,10 @@
         <v>24</v>
       </c>
       <c r="E141" t="s">
+        <v>256</v>
+      </c>
+      <c r="F141" t="s">
         <v>257</v>
-      </c>
-      <c r="F141" t="s">
-        <v>258</v>
       </c>
       <c r="G141">
         <v>766.1</v>
@@ -34439,7 +34436,7 @@
         <v>24</v>
       </c>
       <c r="E142" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F142" t="s">
         <v>173</v>
@@ -34593,10 +34590,10 @@
         <v>24</v>
       </c>
       <c r="E144" t="s">
+        <v>259</v>
+      </c>
+      <c r="F144" t="s">
         <v>260</v>
-      </c>
-      <c r="F144" t="s">
-        <v>261</v>
       </c>
       <c r="G144">
         <v>766</v>
@@ -34670,10 +34667,10 @@
         <v>24</v>
       </c>
       <c r="E145" t="s">
+        <v>261</v>
+      </c>
+      <c r="F145" t="s">
         <v>262</v>
-      </c>
-      <c r="F145" t="s">
-        <v>263</v>
       </c>
       <c r="G145">
         <v>765.9</v>
@@ -34741,13 +34738,13 @@
         <v>0.55714120370370368</v>
       </c>
       <c r="C146" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D146" t="s">
         <v>24</v>
       </c>
       <c r="E146" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F146" t="s">
         <v>163</v>
@@ -34824,10 +34821,10 @@
         <v>24</v>
       </c>
       <c r="E147" t="s">
+        <v>265</v>
+      </c>
+      <c r="F147" t="s">
         <v>266</v>
-      </c>
-      <c r="F147" t="s">
-        <v>267</v>
       </c>
       <c r="G147">
         <v>764.6</v>
@@ -34901,7 +34898,7 @@
         <v>24</v>
       </c>
       <c r="E148" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F148" t="s">
         <v>206</v>
@@ -34978,7 +34975,7 @@
         <v>24</v>
       </c>
       <c r="E149" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F149" t="s">
         <v>186</v>
@@ -35055,10 +35052,10 @@
         <v>24</v>
       </c>
       <c r="E150" t="s">
+        <v>267</v>
+      </c>
+      <c r="F150" t="s">
         <v>268</v>
-      </c>
-      <c r="F150" t="s">
-        <v>269</v>
       </c>
       <c r="G150">
         <v>764.9</v>
@@ -35289,7 +35286,7 @@
         <v>57</v>
       </c>
       <c r="F153" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G153">
         <v>764.9</v>
@@ -35363,10 +35360,10 @@
         <v>24</v>
       </c>
       <c r="E154" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F154" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G154">
         <v>764.9</v>
@@ -35440,10 +35437,10 @@
         <v>24</v>
       </c>
       <c r="E155" t="s">
+        <v>271</v>
+      </c>
+      <c r="F155" t="s">
         <v>272</v>
-      </c>
-      <c r="F155" t="s">
-        <v>273</v>
       </c>
       <c r="G155">
         <v>765</v>
@@ -35517,7 +35514,7 @@
         <v>24</v>
       </c>
       <c r="E156" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F156" t="s">
         <v>153</v>
@@ -35594,7 +35591,7 @@
         <v>24</v>
       </c>
       <c r="E157" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F157" t="s">
         <v>154</v>
@@ -35748,7 +35745,7 @@
         <v>24</v>
       </c>
       <c r="E159" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F159" t="s">
         <v>127</v>
@@ -35825,10 +35822,10 @@
         <v>24</v>
       </c>
       <c r="E160" t="s">
+        <v>275</v>
+      </c>
+      <c r="F160" t="s">
         <v>276</v>
-      </c>
-      <c r="F160" t="s">
-        <v>277</v>
       </c>
       <c r="G160">
         <v>765.7</v>
@@ -35902,7 +35899,7 @@
         <v>24</v>
       </c>
       <c r="E161" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F161" t="s">
         <v>47</v>
@@ -35982,7 +35979,7 @@
         <v>130</v>
       </c>
       <c r="F162" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G162">
         <v>765.8</v>
@@ -36050,13 +36047,13 @@
         <v>0.56421296296296297</v>
       </c>
       <c r="C163" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D163" t="s">
         <v>24</v>
       </c>
       <c r="E163" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F163" t="s">
         <v>227</v>
@@ -36136,7 +36133,7 @@
         <v>132</v>
       </c>
       <c r="F164" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G164">
         <v>762.8</v>
@@ -36213,7 +36210,7 @@
         <v>132</v>
       </c>
       <c r="F165" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G165">
         <v>762.7</v>
@@ -36287,10 +36284,10 @@
         <v>24</v>
       </c>
       <c r="E166" t="s">
+        <v>281</v>
+      </c>
+      <c r="F166" t="s">
         <v>282</v>
-      </c>
-      <c r="F166" t="s">
-        <v>283</v>
       </c>
       <c r="G166">
         <v>762.6</v>
@@ -36364,7 +36361,7 @@
         <v>24</v>
       </c>
       <c r="E167" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F167" t="s">
         <v>90</v>
@@ -36444,7 +36441,7 @@
         <v>187</v>
       </c>
       <c r="F168" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G168">
         <v>762.7</v>
@@ -36521,7 +36518,7 @@
         <v>189</v>
       </c>
       <c r="F169" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G169">
         <v>762.7</v>
@@ -36672,7 +36669,7 @@
         <v>24</v>
       </c>
       <c r="E171" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F171" t="s">
         <v>169</v>
@@ -36749,7 +36746,7 @@
         <v>24</v>
       </c>
       <c r="E172" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F172" t="s">
         <v>38</v>
@@ -36826,10 +36823,10 @@
         <v>24</v>
       </c>
       <c r="E173" t="s">
+        <v>286</v>
+      </c>
+      <c r="F173" t="s">
         <v>287</v>
-      </c>
-      <c r="F173" t="s">
-        <v>288</v>
       </c>
       <c r="G173">
         <v>762.7</v>
@@ -36903,10 +36900,10 @@
         <v>24</v>
       </c>
       <c r="E174" t="s">
+        <v>288</v>
+      </c>
+      <c r="F174" t="s">
         <v>289</v>
-      </c>
-      <c r="F174" t="s">
-        <v>290</v>
       </c>
       <c r="G174">
         <v>762.7</v>
@@ -36980,10 +36977,10 @@
         <v>24</v>
       </c>
       <c r="E175" t="s">
+        <v>290</v>
+      </c>
+      <c r="F175" t="s">
         <v>291</v>
-      </c>
-      <c r="F175" t="s">
-        <v>292</v>
       </c>
       <c r="G175">
         <v>762.7</v>
@@ -37057,10 +37054,10 @@
         <v>24</v>
       </c>
       <c r="E176" t="s">
+        <v>292</v>
+      </c>
+      <c r="F176" t="s">
         <v>293</v>
-      </c>
-      <c r="F176" t="s">
-        <v>294</v>
       </c>
       <c r="G176">
         <v>762.7</v>
@@ -37137,7 +37134,7 @@
         <v>78</v>
       </c>
       <c r="F177" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G177">
         <v>762.7</v>
@@ -37211,7 +37208,7 @@
         <v>24</v>
       </c>
       <c r="E178" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F178" t="s">
         <v>199</v>
@@ -37288,10 +37285,10 @@
         <v>24</v>
       </c>
       <c r="E179" t="s">
+        <v>295</v>
+      </c>
+      <c r="F179" t="s">
         <v>296</v>
-      </c>
-      <c r="F179" t="s">
-        <v>297</v>
       </c>
       <c r="G179">
         <v>762.8</v>
@@ -37365,10 +37362,10 @@
         <v>24</v>
       </c>
       <c r="E180" t="s">
+        <v>297</v>
+      </c>
+      <c r="F180" t="s">
         <v>298</v>
-      </c>
-      <c r="F180" t="s">
-        <v>299</v>
       </c>
       <c r="G180">
         <v>762.7</v>
@@ -37436,13 +37433,13 @@
         <v>0.56983796296296296</v>
       </c>
       <c r="C181" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D181" t="s">
         <v>24</v>
       </c>
       <c r="E181" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F181" t="s">
         <v>86</v>
@@ -37519,7 +37516,7 @@
         <v>24</v>
       </c>
       <c r="E182" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F182" t="s">
         <v>68</v>
@@ -37596,10 +37593,10 @@
         <v>24</v>
       </c>
       <c r="E183" t="s">
+        <v>300</v>
+      </c>
+      <c r="F183" t="s">
         <v>301</v>
-      </c>
-      <c r="F183" t="s">
-        <v>302</v>
       </c>
       <c r="G183">
         <v>763.3</v>
@@ -37676,7 +37673,7 @@
         <v>144</v>
       </c>
       <c r="F184" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G184">
         <v>763.4</v>
@@ -37753,7 +37750,7 @@
         <v>142</v>
       </c>
       <c r="F185" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G185">
         <v>763.3</v>
@@ -37904,7 +37901,7 @@
         <v>24</v>
       </c>
       <c r="E187" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F187" t="s">
         <v>94</v>
@@ -37981,10 +37978,10 @@
         <v>24</v>
       </c>
       <c r="E188" t="s">
+        <v>305</v>
+      </c>
+      <c r="F188" t="s">
         <v>306</v>
-      </c>
-      <c r="F188" t="s">
-        <v>307</v>
       </c>
       <c r="G188">
         <v>763.5</v>
@@ -38058,7 +38055,7 @@
         <v>24</v>
       </c>
       <c r="E189" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F189" t="s">
         <v>56</v>
@@ -38135,10 +38132,10 @@
         <v>24</v>
       </c>
       <c r="E190" t="s">
+        <v>307</v>
+      </c>
+      <c r="F190" t="s">
         <v>308</v>
-      </c>
-      <c r="F190" t="s">
-        <v>309</v>
       </c>
       <c r="G190">
         <v>763.9</v>
@@ -38212,10 +38209,10 @@
         <v>24</v>
       </c>
       <c r="E191" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F191" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G191">
         <v>764</v>
@@ -38289,10 +38286,10 @@
         <v>24</v>
       </c>
       <c r="E192" t="s">
+        <v>310</v>
+      </c>
+      <c r="F192" t="s">
         <v>311</v>
-      </c>
-      <c r="F192" t="s">
-        <v>312</v>
       </c>
       <c r="G192">
         <v>764</v>
@@ -38366,7 +38363,7 @@
         <v>24</v>
       </c>
       <c r="E193" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F193" t="s">
         <v>194</v>
@@ -38446,7 +38443,7 @@
         <v>219</v>
       </c>
       <c r="F194" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G194">
         <v>764</v>
@@ -38520,10 +38517,10 @@
         <v>24</v>
       </c>
       <c r="E195" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F195" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G195">
         <v>764.2</v>
@@ -38597,7 +38594,7 @@
         <v>24</v>
       </c>
       <c r="E196" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F196" t="s">
         <v>199</v>
@@ -38674,10 +38671,10 @@
         <v>24</v>
       </c>
       <c r="E197" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F197" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G197">
         <v>764.3</v>
@@ -38751,10 +38748,10 @@
         <v>24</v>
       </c>
       <c r="E198" t="s">
+        <v>316</v>
+      </c>
+      <c r="F198" t="s">
         <v>317</v>
-      </c>
-      <c r="F198" t="s">
-        <v>318</v>
       </c>
       <c r="G198">
         <v>764.3</v>
@@ -38822,13 +38819,13 @@
         <v>0.55275462962962962</v>
       </c>
       <c r="C199" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D199" t="s">
         <v>24</v>
       </c>
       <c r="E199" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F199" t="s">
         <v>227</v>
@@ -38905,10 +38902,10 @@
         <v>24</v>
       </c>
       <c r="E200" t="s">
+        <v>318</v>
+      </c>
+      <c r="F200" t="s">
         <v>319</v>
-      </c>
-      <c r="F200" t="s">
-        <v>320</v>
       </c>
       <c r="G200">
         <v>762.8</v>
@@ -38985,7 +38982,7 @@
         <v>25</v>
       </c>
       <c r="F201" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G201">
         <v>762.9</v>
@@ -39062,7 +39059,7 @@
         <v>28</v>
       </c>
       <c r="F202" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G202">
         <v>763.1</v>
@@ -39139,7 +39136,7 @@
         <v>53</v>
       </c>
       <c r="F203" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G203">
         <v>762.9</v>
@@ -39213,7 +39210,7 @@
         <v>24</v>
       </c>
       <c r="E204" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F204" t="s">
         <v>32</v>
@@ -39290,7 +39287,7 @@
         <v>24</v>
       </c>
       <c r="E205" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F205" t="s">
         <v>169</v>
@@ -39367,10 +39364,10 @@
         <v>24</v>
       </c>
       <c r="E206" t="s">
+        <v>323</v>
+      </c>
+      <c r="F206" t="s">
         <v>324</v>
-      </c>
-      <c r="F206" t="s">
-        <v>325</v>
       </c>
       <c r="G206">
         <v>763</v>
@@ -39521,7 +39518,7 @@
         <v>24</v>
       </c>
       <c r="E208" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F208" t="s">
         <v>58</v>
@@ -39598,10 +39595,10 @@
         <v>24</v>
       </c>
       <c r="E209" t="s">
+        <v>326</v>
+      </c>
+      <c r="F209" t="s">
         <v>327</v>
-      </c>
-      <c r="F209" t="s">
-        <v>328</v>
       </c>
       <c r="G209">
         <v>763.4</v>
@@ -39675,7 +39672,7 @@
         <v>24</v>
       </c>
       <c r="E210" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F210" t="s">
         <v>109</v>
@@ -39752,10 +39749,10 @@
         <v>24</v>
       </c>
       <c r="E211" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F211" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G211">
         <v>763.5</v>
@@ -39829,10 +39826,10 @@
         <v>24</v>
       </c>
       <c r="E212" t="s">
+        <v>330</v>
+      </c>
+      <c r="F212" t="s">
         <v>331</v>
-      </c>
-      <c r="F212" t="s">
-        <v>332</v>
       </c>
       <c r="G212">
         <v>763.7</v>
@@ -39906,10 +39903,10 @@
         <v>24</v>
       </c>
       <c r="E213" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F213" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G213">
         <v>763.7</v>
@@ -39983,10 +39980,10 @@
         <v>24</v>
       </c>
       <c r="E214" t="s">
+        <v>332</v>
+      </c>
+      <c r="F214" t="s">
         <v>333</v>
-      </c>
-      <c r="F214" t="s">
-        <v>334</v>
       </c>
       <c r="G214">
         <v>763.7</v>
@@ -40060,10 +40057,10 @@
         <v>24</v>
       </c>
       <c r="E215" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F215" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G215">
         <v>763.7</v>
@@ -40140,7 +40137,7 @@
         <v>49</v>
       </c>
       <c r="F216" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G216">
         <v>763.7</v>
@@ -40208,13 +40205,13 @@
         <v>0.56646990740740744</v>
       </c>
       <c r="C217" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D217" t="s">
         <v>24</v>
       </c>
       <c r="E217" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F217" t="s">
         <v>86</v>
@@ -41618,16 +41615,16 @@
         <v>22</v>
       </c>
       <c r="AB1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AM1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AX1" t="s">
+        <v>240</v>
+      </c>
+      <c r="BI1" s="3" t="s">
         <v>241</v>
-      </c>
-      <c r="BI1" s="3" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:70" x14ac:dyDescent="0.3">
@@ -41707,124 +41704,124 @@
         <v>20.73</v>
       </c>
       <c r="AB2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AC2" t="s">
+        <v>238</v>
+      </c>
+      <c r="AD2" t="s">
         <v>239</v>
       </c>
-      <c r="AD2" t="s">
-        <v>240</v>
-      </c>
       <c r="AE2" t="s">
+        <v>242</v>
+      </c>
+      <c r="AF2" t="s">
         <v>243</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>244</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>245</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>246</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>247</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>248</v>
       </c>
-      <c r="AK2" t="s">
-        <v>249</v>
-      </c>
       <c r="AM2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AN2" t="s">
+        <v>238</v>
+      </c>
+      <c r="AO2" t="s">
         <v>239</v>
       </c>
-      <c r="AO2" t="s">
-        <v>240</v>
-      </c>
       <c r="AP2" t="s">
+        <v>242</v>
+      </c>
+      <c r="AQ2" t="s">
         <v>243</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>244</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>245</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>246</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AU2" t="s">
         <v>247</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AV2" t="s">
         <v>248</v>
       </c>
-      <c r="AV2" t="s">
-        <v>249</v>
-      </c>
       <c r="AX2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AY2" t="s">
+        <v>238</v>
+      </c>
+      <c r="AZ2" t="s">
         <v>239</v>
       </c>
-      <c r="AZ2" t="s">
-        <v>240</v>
-      </c>
       <c r="BA2" t="s">
+        <v>242</v>
+      </c>
+      <c r="BB2" t="s">
         <v>243</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BC2" t="s">
         <v>244</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BD2" t="s">
         <v>245</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BE2" t="s">
         <v>246</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BF2" t="s">
         <v>247</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BG2" t="s">
         <v>248</v>
       </c>
-      <c r="BG2" t="s">
-        <v>249</v>
-      </c>
       <c r="BI2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="BJ2" t="s">
+        <v>238</v>
+      </c>
+      <c r="BK2" t="s">
         <v>239</v>
       </c>
-      <c r="BK2" t="s">
-        <v>240</v>
-      </c>
       <c r="BL2" t="s">
+        <v>242</v>
+      </c>
+      <c r="BM2" t="s">
         <v>243</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="BN2" t="s">
         <v>244</v>
       </c>
-      <c r="BN2" t="s">
+      <c r="BO2" t="s">
         <v>245</v>
       </c>
-      <c r="BO2" t="s">
+      <c r="BP2" t="s">
         <v>246</v>
       </c>
-      <c r="BP2" t="s">
+      <c r="BQ2" t="s">
         <v>247</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="BR2" t="s">
         <v>248</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:70" x14ac:dyDescent="0.3">
@@ -43404,7 +43401,7 @@
         <v>40.61</v>
       </c>
       <c r="AB11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AC11">
         <v>20.5</v>
@@ -43420,11 +43417,11 @@
       </c>
       <c r="AK11" s="4"/>
       <c r="AM11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AV11" s="4"/>
       <c r="AX11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AY11">
         <v>27.8</v>
@@ -43442,7 +43439,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="BI11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="BJ11">
         <v>26.8</v>
@@ -43538,7 +43535,7 @@
         <v>25.32</v>
       </c>
       <c r="AB12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AC12">
         <v>19.7</v>
@@ -43554,7 +43551,7 @@
       </c>
       <c r="AK12" s="4"/>
       <c r="AM12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AN12">
         <v>18.3</v>
@@ -43569,7 +43566,7 @@
         <v>0.42</v>
       </c>
       <c r="AX12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AY12">
         <v>27</v>
@@ -43585,7 +43582,7 @@
       </c>
       <c r="BG12" s="5"/>
       <c r="BI12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="BJ12">
         <v>26.3</v>

</xml_diff>